<commit_message>
Filmabrechnungen welche aus anderen Abrechnungsperioden entstanden sind entfehrnt
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wagne\Dropbox\Kino\Rechnungen, Einnahmen und Ausgaben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF60B47-D941-4D16-BBDD-2257AE68415A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC19161-2C8C-42FD-9B7D-8F2E2B21A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="4065" yWindow="3300" windowWidth="29475" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Filmausgaben" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Projektbeitrag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schulden aus anderen Abrechnungsperioden </t>
   </si>
 </sst>
 </file>
@@ -319,6 +322,12 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -326,12 +335,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -365,8 +368,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5109FEF6-8EB9-418D-9444-3A01886A72B5}" name="Table1" displayName="Table1" ref="A1:H4" totalsRowShown="0">
-  <autoFilter ref="A1:H4" xr:uid="{5109FEF6-8EB9-418D-9444-3A01886A72B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5109FEF6-8EB9-418D-9444-3A01886A72B5}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{5109FEF6-8EB9-418D-9444-3A01886A72B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D3E4C346-5641-4ACE-BE6E-787FF210B4F4}" name="Bezeichnung"/>
     <tableColumn id="2" xr3:uid="{C74ECB02-FB43-4FB6-AD99-9865B4318150}" name="Rechnungsdatum" dataDxfId="10"/>
@@ -387,12 +390,12 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{14F4F8C5-55F3-473E-9937-8D0B7D552E7E}" name="Bezeichnung"/>
     <tableColumn id="9" xr3:uid="{08E3E686-942A-44EF-B27E-3FE86295855D}" name="Kategorie"/>
-    <tableColumn id="2" xr3:uid="{150155FD-26CC-46D0-A27B-59EA4645C5CC}" name="Rechnungsdatum" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{35B5C014-5D17-48B7-9F63-677F9270FF60}" name="Betrag" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{150155FD-26CC-46D0-A27B-59EA4645C5CC}" name="Rechnungsdatum" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{35B5C014-5D17-48B7-9F63-677F9270FF60}" name="Betrag" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{ADC4C0E0-A7EA-4AFB-901E-6392865FA73A}" name="Firmennamen"/>
     <tableColumn id="5" xr3:uid="{C65688D5-41D8-437C-9C57-8C2751C5B1B9}" name="Adresse"/>
     <tableColumn id="6" xr3:uid="{27E43FFA-FA55-425E-A213-9BD13C8F6254}" name="Referenz"/>
-    <tableColumn id="7" xr3:uid="{10A8576E-804F-45CC-A7BA-BA671FF72F24}" name="Rechnungsnummer" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{10A8576E-804F-45CC-A7BA-BA671FF72F24}" name="Rechnungsnummer" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{E3354F54-F1AF-4001-AF7B-A661D76F7FAC}" name="SpielDatum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -404,12 +407,12 @@
   <autoFilter ref="A1:G7" xr:uid="{180DF3BF-586A-489C-84B8-C4618CD829F6}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F238A2B1-EDB6-47A0-885E-5CEEFF41F1CF}" name="Bezeichnung"/>
-    <tableColumn id="2" xr3:uid="{2177CF86-5EB2-4966-9940-7F31F280BF61}" name="Datum" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{DD645600-C5EC-4AB1-8AE1-7605051A2066}" name="Betrag" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2177CF86-5EB2-4966-9940-7F31F280BF61}" name="Datum" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DD645600-C5EC-4AB1-8AE1-7605051A2066}" name="Betrag" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{822BB147-F960-4922-A447-9B097046BFC7}" name="Firmennamen"/>
     <tableColumn id="5" xr3:uid="{7EC3E0C6-7422-492C-82ED-2D8E00F73F8D}" name="Adresse"/>
     <tableColumn id="6" xr3:uid="{283A3E60-3B55-4B6F-93F7-1566169ACFF6}" name="Referenz"/>
-    <tableColumn id="7" xr3:uid="{B4FB147A-04B0-4D58-A6A4-685D055BABDA}" name="Rechnungsnummer" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B4FB147A-04B0-4D58-A6A4-685D055BABDA}" name="Rechnungsnummer" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -420,8 +423,8 @@
   <autoFilter ref="A1:G6" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
-    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{EC0FDCA3-B34E-4378-9B61-6671AF218B0B}" name="Firmennamen"/>
     <tableColumn id="8" xr3:uid="{359B982D-E085-4831-8FE0-859B1B4314AD}" name="Adresse"/>
     <tableColumn id="10" xr3:uid="{02367AEA-A5FC-4D0B-90AF-F9D0D56EB4A0}" name="Rechnungsnummer"/>
@@ -728,25 +731,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6432BC27-B3C4-4504-9F14-2864DE81520F}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -772,81 +775,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>44914</v>
+        <v>44908</v>
       </c>
       <c r="C2" s="4">
-        <v>176.65</v>
+        <v>211.1</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45044</v>
       </c>
       <c r="H2" s="1">
-        <v>44905</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44914</v>
-      </c>
-      <c r="C3" s="4">
-        <v>112.7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1">
-        <v>44912</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44908</v>
-      </c>
-      <c r="C4" s="4">
-        <v>211.1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2">
-        <v>45044</v>
-      </c>
-      <c r="H4" s="1">
         <v>45262</v>
       </c>
     </row>
@@ -860,26 +811,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CCE82D-AE8A-46F8-BC0A-7BF5F2C85660}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -937,7 +888,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -963,7 +914,7 @@
         <v>63216</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -989,7 +940,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +966,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1038,7 +989,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1059,7 +1010,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1079,6 +1030,64 @@
         <v>60</v>
       </c>
       <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44914</v>
+      </c>
+      <c r="D9" s="4">
+        <v>176.65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44914</v>
+      </c>
+      <c r="D10" s="4">
+        <v>112.7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1">
+        <v>44912</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1096,18 +1105,18 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>27696257</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>27719686</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1213,10 +1222,10 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="4"/>
       <c r="G7" s="2"/>
@@ -1237,18 +1246,18 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1271,7 +1280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Rechnungen von anderen Abrechnungsperioden korrekt kategorisiert
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC19161-2C8C-42FD-9B7D-8F2E2B21A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72A8928-53C3-4DD1-A62D-188CCBD6793D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="3300" windowWidth="29475" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="3720" yWindow="2955" windowWidth="29475" windowHeight="15345" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Filmausgaben" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
     <t>Projektbeitrag</t>
   </si>
   <si>
-    <t xml:space="preserve">Schulden aus anderen Abrechnungsperioden </t>
+    <t xml:space="preserve">Rechnungen aus anderen Abrechnungsperioden </t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6432BC27-B3C4-4504-9F14-2864DE81520F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -813,14 +813,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CCE82D-AE8A-46F8-BC0A-7BF5F2C85660}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Einnahme und Ausgaben korrrigiert
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95C0E1F-0B00-4361-BEE3-D3261EA13795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C7E3AD-8EDE-4BFC-9411-5A4B8744D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="3720" yWindow="2955" windowWidth="29475" windowHeight="15345" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -278,15 +278,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -294,22 +300,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -318,12 +354,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -344,12 +374,12 @@
   <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
-    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{0C538012-5D92-4E64-B81F-85CAF66FE963}" name="Firmennamen"/>
     <tableColumn id="5" xr3:uid="{528DBE91-75A0-4B49-8AC8-06D027A50035}" name="Adresse"/>
     <tableColumn id="6" xr3:uid="{4B5E1481-D849-49CA-8C98-0F7393B356B7}" name="Referenz"/>
-    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -357,18 +387,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G6" totalsRowShown="0">
-  <autoFilter ref="A1:G6" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
     <tableColumn id="2" xr3:uid="{4A3D2615-9D9C-4A35-9563-6454B477091D}" name="Bezeichnung"/>
-    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{EC0FDCA3-B34E-4378-9B61-6671AF218B0B}" name="Firmennamen"/>
     <tableColumn id="8" xr3:uid="{359B982D-E085-4831-8FE0-859B1B4314AD}" name="Adresse"/>
     <tableColumn id="10" xr3:uid="{02367AEA-A5FC-4D0B-90AF-F9D0D56EB4A0}" name="Rechnungsnummer"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -671,24 +701,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -717,7 +747,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -743,7 +773,7 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -769,7 +799,7 @@
         <v>27696257</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -795,7 +825,7 @@
         <v>27719686</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -818,7 +848,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -840,7 +870,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -861,7 +891,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -887,7 +917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -913,7 +943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -934,7 +964,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -963,7 +993,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -992,7 +1022,7 @@
         <v>44912</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1018,7 +1048,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1044,7 +1074,7 @@
         <v>63216</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1077,24 +1107,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1117,7 +1147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1140,7 +1170,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1160,7 +1190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1181,7 +1211,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1198,7 +1228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1214,6 +1244,27 @@
       <c r="E6" t="s">
         <v>68</v>
       </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8">
+        <v>45268</v>
+      </c>
+      <c r="D7" s="9">
+        <v>54.48</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Einnahmen und Ausgaben korrigiert
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C7E3AD-8EDE-4BFC-9411-5A4B8744D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A12D8EA-DD87-4B65-A5BB-4839B721E189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2955" windowWidth="29475" windowHeight="15345" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="3720" yWindow="2955" windowWidth="29475" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Zweifel Gutschrift Kiosk-Retouren</t>
-  </si>
-  <si>
-    <t>91 59710 00000 56775 52771 96860</t>
   </si>
   <si>
     <t>Rechnung Filmvermietung Ein Schotte macht noch keinen Sommer</t>
@@ -331,10 +328,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,8 +366,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I14" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
@@ -699,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -744,12 +741,12 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -775,7 +772,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -801,172 +798,175 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1">
-        <v>45268</v>
+        <v>45243</v>
       </c>
       <c r="D4" s="4">
-        <v>-54.48</v>
+        <v>422.6</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2">
-        <v>27719686</v>
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1">
-        <v>45243</v>
+        <v>45231</v>
       </c>
       <c r="D5" s="4">
-        <v>422.6</v>
+        <f>45*2.3</f>
+        <v>103.49999999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1">
-        <v>45231</v>
+        <v>45153</v>
       </c>
       <c r="D6" s="4">
-        <f>45*2.3</f>
-        <v>103.49999999999999</v>
+        <v>609.79999999999995</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
-        <v>45153</v>
+        <v>45180</v>
       </c>
       <c r="D7" s="4">
-        <v>609.79999999999995</v>
+        <v>3752.6</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1">
         <v>45180</v>
       </c>
       <c r="D8" s="4">
-        <v>3752.6</v>
+        <v>542.4</v>
       </c>
       <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1">
-        <v>45180</v>
+        <v>45291</v>
       </c>
       <c r="D9" s="4">
-        <v>542.4</v>
+        <v>12000</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>45291</v>
+        <v>44914</v>
       </c>
       <c r="D10" s="4">
-        <v>12000</v>
+        <v>176.65</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1">
+        <v>44905</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -975,7 +975,7 @@
         <v>44914</v>
       </c>
       <c r="D11" s="4">
-        <v>176.65</v>
+        <v>112.7</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -987,39 +987,36 @@
         <v>9</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" s="1">
-        <v>44905</v>
+        <v>44912</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>44914</v>
+        <v>45240</v>
       </c>
       <c r="D12" s="4">
-        <v>112.7</v>
+        <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="I12" s="1">
-        <v>44912</v>
+        <v>45248</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,74 +1024,48 @@
         <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>45240</v>
+        <v>45107</v>
       </c>
       <c r="D13" s="4">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="1">
-        <v>45248</v>
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="2">
+        <v>63216</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1">
-        <v>45107</v>
+        <v>45244</v>
       </c>
       <c r="D14" s="4">
-        <v>20</v>
+        <v>153.69999999999999</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="2">
-        <v>63216</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="1">
-        <v>45244</v>
-      </c>
-      <c r="D15" s="4">
-        <v>153.69999999999999</v>
-      </c>
-      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H14" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1109,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1126,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1149,10 +1120,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5">
         <v>45260</v>
@@ -1161,21 +1132,21 @@
         <v>58.58</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="5">
         <v>45248</v>
@@ -1184,18 +1155,18 @@
         <v>800</v>
       </c>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
         <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="5">
         <v>45255</v>
@@ -1204,19 +1175,19 @@
         <v>250</v>
       </c>
       <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
         <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="5">
         <v>45265</v>
@@ -1225,15 +1196,15 @@
         <v>14380</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5">
         <v>45265</v>
@@ -1242,12 +1213,12 @@
         <v>10000</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Neue Rechnung eingefügt Fliegende Klassenzimmer
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5BC944-42BA-4D6E-93E4-9D485DCCFE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE9A854-0E34-4D24-87A3-F981786421DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2955" windowWidth="29475" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>Werbung Zeitungsinserat Wynentaler</t>
+  </si>
+  <si>
+    <t>Rechnung Film Das Fliegende Klassenzimmer</t>
+  </si>
+  <si>
+    <t>DCM Film Distribution (Schweiz) GmbH</t>
+  </si>
+  <si>
+    <t>96 57660 00000 00000 00301 57626</t>
+  </si>
+  <si>
+    <t>03015762</t>
   </si>
 </sst>
 </file>
@@ -366,8 +378,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I14" totalsRowShown="0">
-  <autoFilter ref="A1:I14" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
@@ -696,26 +708,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -744,7 +756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -770,7 +782,7 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -796,7 +808,7 @@
         <v>27696257</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -819,7 +831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -841,7 +853,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -862,7 +874,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -888,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -914,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -935,7 +947,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -964,7 +976,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -993,7 +1005,7 @@
         <v>44912</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1019,7 +1031,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1045,7 +1057,7 @@
         <v>63216</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1066,6 +1078,35 @@
       </c>
       <c r="H14" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45279</v>
+      </c>
+      <c r="D15" s="4">
+        <v>161.55000000000001</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1">
+        <v>45242</v>
       </c>
     </row>
   </sheetData>
@@ -1084,18 +1125,18 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1118,7 +1159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1141,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1161,7 +1202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1182,7 +1223,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1199,7 +1240,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1216,7 +1257,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Abrechnung hinzugefügt: Das fliegende Klassenzimmer
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE9A854-0E34-4D24-87A3-F981786421DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B818F01-1B82-4FB9-BD3B-D9817B38D0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -710,24 +710,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -756,7 +756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -782,7 +782,7 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -808,7 +808,7 @@
         <v>27696257</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -831,7 +831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -900,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -926,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -947,7 +947,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -976,7 +976,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>44912</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>63216</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1125,18 +1125,18 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Sozialleistungen Gehaltszahlungen: Fakto 1.1 auf Bruttogehalt
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C03BAD-A571-402D-985A-2A08EB7D5616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA2FD4-0B95-4F0A-B460-E0C987925152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="3135" yWindow="2625" windowWidth="29010" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Gehaltszahlung Projektleitung</t>
+  </si>
+  <si>
+    <t>Lohn</t>
   </si>
 </sst>
 </file>
@@ -714,7 +717,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1117,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>77</v>
@@ -1123,8 +1126,8 @@
         <v>45010</v>
       </c>
       <c r="D16" s="4">
-        <f>1500*1.2</f>
-        <v>1800</v>
+        <f>1500*1.1</f>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E16" t="s">
         <v>50</v>
@@ -1145,8 +1148,8 @@
         <v>45041</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" ref="D17:D25" si="0">1500*1.2</f>
-        <v>1800</v>
+        <f t="shared" ref="D17:D25" si="0">1500*1.1</f>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E17" t="s">
         <v>50</v>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
@@ -1190,7 +1193,7 @@
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E19" t="s">
         <v>50</v>
@@ -1212,7 +1215,7 @@
       </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E20" t="s">
         <v>50</v>
@@ -1234,7 +1237,7 @@
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E21" t="s">
         <v>50</v>
@@ -1256,7 +1259,7 @@
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E22" t="s">
         <v>50</v>
@@ -1278,7 +1281,7 @@
       </c>
       <c r="D23" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E23" t="s">
         <v>50</v>
@@ -1300,7 +1303,7 @@
       </c>
       <c r="D24" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E24" t="s">
         <v>50</v>
@@ -1322,7 +1325,7 @@
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>1650.0000000000002</v>
       </c>
       <c r="E25" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Neue Kategorie Ausgaben: Personalaufwand
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA2FD4-0B95-4F0A-B460-E0C987925152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2AE542-A1B2-4EFD-AD7A-661755EBCB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3135" yWindow="2625" windowWidth="29010" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -273,7 +273,7 @@
     <t>Gehaltszahlung Projektleitung</t>
   </si>
   <si>
-    <t>Lohn</t>
+    <t>Personalaufwand</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>77</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>77</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>77</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
         <v>77</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Neue Kategorie Personalkosten implementiert
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2AE542-A1B2-4EFD-AD7A-661755EBCB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F03B47D-3A96-44F8-B58C-E9CF1B69F1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2625" windowWidth="29010" windowHeight="15345" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgaben" sheetId="5" r:id="rId1"/>
@@ -717,7 +717,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Beitrag Aargauer Kuratorium 2023
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDF9A4-FF67-4FD7-AA81-AA2ED543F3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA44A616-F7A1-488F-B318-17B2C4227E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -270,10 +270,34 @@
     <t>03015762</t>
   </si>
   <si>
+    <t>Rechnung Ingeborg Bachmann</t>
+  </si>
+  <si>
+    <t>Filmcoopi Zürich AG</t>
+  </si>
+  <si>
+    <t>Heinrichstrasse 114, 8005 Zürich</t>
+  </si>
+  <si>
+    <t>93 64950 00000 00000 00008 38954</t>
+  </si>
+  <si>
+    <t>00083895</t>
+  </si>
+  <si>
+    <t>93 64950 00000 00000 00008 38946</t>
+  </si>
+  <si>
+    <t>00083894</t>
+  </si>
+  <si>
+    <t>Personalaufwand</t>
+  </si>
+  <si>
     <t>Gehaltszahlung Projektleitung</t>
   </si>
   <si>
-    <t>Personalaufwand</t>
+    <t>Aargauer Kuratorium</t>
   </si>
 </sst>
 </file>
@@ -384,8 +408,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G8" totalsRowShown="0">
+  <autoFilter ref="A1:G8" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
     <tableColumn id="2" xr3:uid="{4A3D2615-9D9C-4A35-9563-6454B477091D}" name="Bezeichnung"/>
@@ -400,8 +424,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I25" totalsRowShown="0">
-  <autoFilter ref="A1:I25" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I26" totalsRowShown="0">
+  <autoFilter ref="A1:I26" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
@@ -714,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,6 +897,23 @@
       </c>
       <c r="G7" s="7"/>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45265</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -883,10 +924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A18" sqref="A18:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,60 +1327,74 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="1">
-        <v>45010</v>
+        <v>45291</v>
       </c>
       <c r="D16" s="4">
-        <f>1710*1.1</f>
-        <v>1881.0000000000002</v>
+        <v>127.05</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="1">
+        <v>45267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
         <v>77</v>
       </c>
       <c r="C17" s="1">
+        <v>45291</v>
+      </c>
+      <c r="D17" s="4">
+        <v>231.55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="1">
+        <v>45256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="1">
         <v>45041</v>
       </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D25" si="0">1710*1.1</f>
-        <v>1881.0000000000002</v>
-      </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="1">
-        <v>45071</v>
-      </c>
       <c r="D18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D18:D26" si="0">1710*1.1</f>
         <v>1881.0000000000002</v>
       </c>
       <c r="E18" t="s">
@@ -1350,15 +1405,15 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1">
-        <v>45102</v>
+        <v>45071</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
@@ -1372,15 +1427,15 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1">
-        <v>45132</v>
+        <v>45102</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
@@ -1394,15 +1449,15 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1">
-        <v>45163</v>
+        <v>45132</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
@@ -1416,15 +1471,15 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1">
-        <v>45194</v>
+        <v>45163</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
@@ -1438,15 +1493,15 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1">
-        <v>45224</v>
+        <v>45194</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="0"/>
@@ -1460,15 +1515,15 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1">
-        <v>45255</v>
+        <v>45224</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="0"/>
@@ -1482,15 +1537,15 @@
       </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1">
-        <v>45285</v>
+        <v>45255</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
@@ -1503,6 +1558,28 @@
         <v>51</v>
       </c>
       <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45285</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>1881.0000000000002</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dropdown in Einnahmen und Ausgaben eingefügt
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub 2024\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4BF8FE-3507-45A2-96F0-54E49C34E50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D8BB6E-B9DB-49AF-A157-8230F4A03D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -142,21 +142,9 @@
     <t>Stefan Jablonski</t>
   </si>
   <si>
-    <t>Film</t>
-  </si>
-  <si>
-    <t>drop down</t>
-  </si>
-  <si>
-    <t>Event</t>
-  </si>
-  <si>
     <t>Verleiher</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Fiktive Verleiherrechnung</t>
   </si>
   <si>
@@ -164,6 +152,15 @@
   </si>
   <si>
     <t>Fiktivstrasse 38, 8005 NichtZürich</t>
+  </si>
+  <si>
+    <t>Eventausgaben</t>
+  </si>
+  <si>
+    <t>drop down Ausgaben</t>
+  </si>
+  <si>
+    <t>drop down Einnahmen</t>
   </si>
 </sst>
 </file>
@@ -197,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -225,11 +222,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,11 +268,88 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -285,8 +387,8 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
     <tableColumn id="2" xr3:uid="{4A3D2615-9D9C-4A35-9563-6454B477091D}" name="Bezeichnung"/>
-    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{EC0FDCA3-B34E-4378-9B61-6671AF218B0B}" name="Firmennamen"/>
     <tableColumn id="8" xr3:uid="{359B982D-E085-4831-8FE0-859B1B4314AD}" name="Adresse"/>
     <tableColumn id="10" xr3:uid="{02367AEA-A5FC-4D0B-90AF-F9D0D56EB4A0}" name="Rechnungsnummer"/>
@@ -296,32 +398,47 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:J26" totalsRowShown="0">
-  <autoFilter ref="A1:J26" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I26" totalsRowShown="0">
+  <autoFilter ref="A1:I26" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I26">
-    <sortCondition ref="C1:C26"/>
+    <sortCondition ref="D1:D26"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
+    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
-    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{0C538012-5D92-4E64-B81F-85CAF66FE963}" name="Firmennamen"/>
     <tableColumn id="5" xr3:uid="{528DBE91-75A0-4B49-8AC8-06D027A50035}" name="Adresse"/>
     <tableColumn id="6" xr3:uid="{4B5E1481-D849-49CA-8C98-0F7393B356B7}" name="Referenz"/>
-    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum"/>
-    <tableColumn id="10" xr3:uid="{F62F2DC3-467E-4788-B697-6B13A0609FEF}" name="Event"/>
+    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0556C6D9-61AE-47D0-BCA8-925AD93BDF07}" name="Table1" displayName="Table1" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4" xr:uid="{0556C6D9-61AE-47D0-BCA8-925AD93BDF07}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0556C6D9-61AE-47D0-BCA8-925AD93BDF07}" name="Table1" displayName="Table1" ref="A1:A8" totalsRowShown="0">
+  <autoFilter ref="A1:A8" xr:uid="{0556C6D9-61AE-47D0-BCA8-925AD93BDF07}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A8">
+    <sortCondition ref="A1:A8"/>
+  </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CC621E62-0BE4-4ADB-B21D-45F38B2D8B9A}" name="drop down"/>
+    <tableColumn id="1" xr3:uid="{CC621E62-0BE4-4ADB-B21D-45F38B2D8B9A}" name="drop down Ausgaben"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C381996-4C8D-47B9-A3E8-3D58D82C2B8C}" name="Table2" displayName="Table2" ref="D1:D8" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="2">
+  <autoFilter ref="D1:D8" xr:uid="{0C381996-4C8D-47B9-A3E8-3D58D82C2B8C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D8">
+    <sortCondition ref="D1:D8"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B36775E4-4356-40D0-B093-06914372A555}" name="drop down Einnahmen" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,572 +881,500 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0F14738-253F-45AA-AA13-7D0E4CE09F27}">
+          <x14:formula1>
+            <xm:f>dropdown!$D$2:$D$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45311</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>45311</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>75.849999999999994</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1">
-        <v>45311</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45312</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>45312</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>48.5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1">
-        <v>45312</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>45316</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>34.5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>45316</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:D16" si="0">1140*1.1</f>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E16" si="0">1140*1.1</f>
         <v>1254</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>45347</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>45376</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="1"/>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>45407</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="J8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>45437</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="J9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>45468</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="J10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>45498</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="J11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>45529</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="J12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>45560</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="J13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>45590</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>9</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="J14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>45621</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>9</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="J15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>45651</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>45657</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
         <v>12000</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="J17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="1">
+        <v>45311</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1">
         <v>45322</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>250.85</v>
       </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
       <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="1">
-        <v>45311</v>
-      </c>
-      <c r="J18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-      <c r="H19" s="2"/>
-      <c r="J19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-      <c r="D20" s="4"/>
-      <c r="H20" s="2"/>
-      <c r="J20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
-      <c r="D21" s="4"/>
-      <c r="H21" s="2"/>
-      <c r="J21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-      <c r="D22" s="4"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="1"/>
-      <c r="J22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-      <c r="D23" s="4"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="1"/>
-      <c r="J23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
-      <c r="D24" s="4"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C25" s="1"/>
-      <c r="D25" s="4"/>
-      <c r="H25" s="2"/>
-      <c r="J25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C26" s="1"/>
-      <c r="D26" s="4"/>
-      <c r="H26" s="2"/>
-      <c r="J26" t="s">
-        <v>38</v>
-      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="1"/>
+      <c r="E19" s="4"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="1"/>
+      <c r="E20" s="4"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="1"/>
+      <c r="E21" s="4"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="4"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="4"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="E24" s="4"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="1"/>
+      <c r="E25" s="4"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="1"/>
+      <c r="E26" s="4"/>
+      <c r="I26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4486DEF-A1C9-4053-A4FF-2511D36CC586}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{551055D3-EB54-4023-842C-CF79CAE47FBC}">
           <x14:formula1>
-            <xm:f>dropdown!$A$2:$A$4</xm:f>
+            <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J26</xm:sqref>
+          <xm:sqref>A2:A26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1339,41 +1384,87 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFEBA5D-FF22-4032-BB29-794CF56A632B}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kategorien mit drop down eingeführt
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub 2024\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA0731-6561-4040-ABD1-A3A6E1793E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F724620A-3297-43EE-A18E-80851BB995F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -626,18 +626,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -677,7 +677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -691,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -702,7 +702,7 @@
         <v>45260</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -713,7 +713,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -740,7 +740,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -780,23 +780,23 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -825,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -849,7 +849,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -913,7 +913,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -935,7 +935,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -957,7 +957,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -979,7 +979,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>45322</v>
       </c>
       <c r="E18" s="4">
-        <v>250.85</v>
+        <v>426.6</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
@@ -1200,42 +1200,42 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="4"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="4"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="4"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="4"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="I26" s="2"/>
@@ -1269,47 +1269,47 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Neuer Eintrag 28.01.24 Gipfeli
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA052E6-694B-45B1-A9B1-2F8717972277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1F4510-8D7A-4800-9BE0-A2D8BF54C184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="42">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">Kaffee und Pocorn </t>
+  </si>
+  <si>
+    <t>Gipfeli</t>
+  </si>
+  <si>
+    <t>Schulz Bäckerei</t>
   </si>
 </sst>
 </file>
@@ -626,7 +632,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,6 +766,23 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45319</v>
+      </c>
+      <c r="D9" s="4">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
Update Einnahmen Ausgaben 24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757FE62A-CFF4-4280-A160-6587DBBAFB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861FC5E2-CD91-45D8-818B-22F17812B6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -61,12 +61,6 @@
     <t>Rechnungsnummer</t>
   </si>
   <si>
-    <t>Zweifel Gutschrift Kiosk-Retouren</t>
-  </si>
-  <si>
-    <t>Werbeeinnahmen für den Monat November</t>
-  </si>
-  <si>
     <t>Nadia Wagner</t>
   </si>
   <si>
@@ -103,15 +97,6 @@
     <t>Kiosk</t>
   </si>
   <si>
-    <t>Projektbeitrag Stiftung Lebensraum Aargau</t>
-  </si>
-  <si>
-    <t>Vermietung Homberg Apotheke</t>
-  </si>
-  <si>
-    <t>Vermietung Geburtstag Filliger</t>
-  </si>
-  <si>
     <t>Spieldatum</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
   </si>
   <si>
     <t>Schulz Bäckerei</t>
-  </si>
-  <si>
-    <t>Vermutete Einnahmen</t>
   </si>
   <si>
     <t>Zweifel Bestellung Januar</t>
@@ -270,21 +252,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -292,44 +268,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +319,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
-    <sortCondition ref="E1:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G3">
+    <sortCondition ref="E1:E3"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
@@ -719,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -761,10 +710,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5">
         <v>45265</v>
@@ -773,15 +722,15 @@
         <v>12000</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>45631</v>
@@ -790,96 +739,7 @@
         <v>12000</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
-        <v>45260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5">
-        <v>45248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5">
-        <v>45255</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10">
-        <v>45265</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="9">
-        <v>45268</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="5">
-        <v>45657</v>
-      </c>
-      <c r="D9" s="4">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5">
-        <v>45657</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3000</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +754,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A14</xm:sqref>
+          <xm:sqref>A2:A7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -906,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -925,10 +785,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -954,13 +814,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>45311</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1">
         <v>45311</v>
@@ -969,23 +829,23 @@
         <v>75.849999999999994</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>45312</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>45312</v>
@@ -994,17 +854,17 @@
         <v>48.5</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>45316</v>
@@ -1013,20 +873,20 @@
         <v>34.5</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>45316</v>
@@ -1036,20 +896,20 @@
         <v>1254</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>45347</v>
@@ -1059,20 +919,20 @@
         <v>1254</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>45376</v>
@@ -1082,20 +942,20 @@
         <v>1254</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>45407</v>
@@ -1105,20 +965,20 @@
         <v>1254</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>45437</v>
@@ -1128,20 +988,20 @@
         <v>1254</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
         <v>45468</v>
@@ -1151,20 +1011,20 @@
         <v>1254</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>45498</v>
@@ -1174,20 +1034,20 @@
         <v>1254</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>45529</v>
@@ -1197,20 +1057,20 @@
         <v>1254</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>45560</v>
@@ -1220,20 +1080,20 @@
         <v>1254</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1">
         <v>45590</v>
@@ -1243,20 +1103,20 @@
         <v>1254</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1">
         <v>45621</v>
@@ -1266,20 +1126,20 @@
         <v>1254</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1">
         <v>45651</v>
@@ -1289,20 +1149,20 @@
         <v>1254</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1">
         <v>45657</v>
@@ -1311,20 +1171,20 @@
         <v>14400</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1">
         <v>45331</v>
@@ -1333,24 +1193,24 @@
         <v>101</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1">
         <v>45316</v>
@@ -1359,23 +1219,23 @@
         <v>32.700000000000003</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5">
         <v>45319</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5">
         <v>45319</v>
@@ -1384,20 +1244,20 @@
         <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1">
         <v>45311</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1">
         <v>45330</v>
@@ -1406,24 +1266,24 @@
         <v>423.5</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1">
         <v>45330</v>
@@ -1432,27 +1292,27 @@
         <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>45312</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1">
         <v>45329</v>
@@ -1461,24 +1321,24 @@
         <v>276.3</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1">
         <v>45329</v>
@@ -1487,24 +1347,24 @@
         <v>35.049999999999997</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1">
         <v>44895</v>
@@ -1513,10 +1373,10 @@
         <v>15.75</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2">
@@ -1525,13 +1385,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>45316</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1">
         <v>45321</v>
@@ -1540,21 +1400,21 @@
         <v>194.6</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="4"/>
@@ -1603,42 +1463,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eventausgaben = neu "Event"
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8CB40D-04B3-45DD-A561-B7193EC1BAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F9C6C6-57A1-41B5-91BF-7375D3AE1CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Verleiher</t>
   </si>
   <si>
-    <t>Eventausgaben</t>
-  </si>
-  <si>
     <t>drop down</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>00084603</t>
+  </si>
+  <si>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -768,7 +768,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +815,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1">
         <v>45311</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1">
         <v>45312</v>
@@ -862,13 +862,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5">
         <v>45319</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5">
         <v>45319</v>
@@ -877,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -909,7 +909,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1">
         <v>45331</v>
@@ -918,16 +918,16 @@
         <v>101</v>
       </c>
       <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1">
         <v>45316</v>
@@ -957,7 +957,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1">
         <v>45316</v>
@@ -980,7 +980,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1">
         <v>45347</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1">
         <v>45330</v>
@@ -1012,24 +1012,24 @@
         <v>100</v>
       </c>
       <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1">
         <v>45329</v>
@@ -1038,24 +1038,24 @@
         <v>35.049999999999997</v>
       </c>
       <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
       <c r="H11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1">
         <v>44895</v>
@@ -1064,10 +1064,10 @@
         <v>15.75</v>
       </c>
       <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2">
@@ -1082,7 +1082,7 @@
         <v>45311</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1">
         <v>45330</v>
@@ -1091,16 +1091,16 @@
         <v>423.5</v>
       </c>
       <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
         <v>35</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1111,7 +1111,7 @@
         <v>45312</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1">
         <v>45329</v>
@@ -1120,16 +1120,16 @@
         <v>276.3</v>
       </c>
       <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1140,7 +1140,7 @@
         <v>45316</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1">
         <v>45321</v>
@@ -1149,24 +1149,24 @@
         <v>194.6</v>
       </c>
       <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" t="s">
         <v>54</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1">
         <v>45316</v>
@@ -1178,17 +1178,17 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1">
         <v>45347</v>
@@ -1200,7 +1200,7 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1213,7 +1213,7 @@
         <v>45333</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1">
         <v>45337</v>
@@ -1222,16 +1222,16 @@
         <v>192.45</v>
       </c>
       <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
         <v>67</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>68</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1263,7 +1263,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,12 +1273,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1293,7 +1293,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Planet Hora Einnahmen und Ausgaben
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8CB40D-04B3-45DD-A561-B7193EC1BAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCFE551-2E71-4F43-88CD-3476D9B66211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -251,6 +251,27 @@
   </si>
   <si>
     <t>00084603</t>
+  </si>
+  <si>
+    <t>Film: Planet Hora</t>
+  </si>
+  <si>
+    <t>Theater Hora</t>
+  </si>
+  <si>
+    <t>Plakate &amp; Flyer Planet Hora</t>
+  </si>
+  <si>
+    <t>L'equippe visuelle</t>
+  </si>
+  <si>
+    <t>Stiftung Lebenshilfe</t>
+  </si>
+  <si>
+    <t>Reinach AG</t>
+  </si>
+  <si>
+    <t>Beitrag Stiftung Lebenshilfe</t>
   </si>
 </sst>
 </file>
@@ -356,8 +377,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I18" totalsRowShown="0">
-  <autoFilter ref="A1:I18" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I20" totalsRowShown="0">
+  <autoFilter ref="A1:I20" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I16">
     <sortCondition ref="A1:A16"/>
   </sortState>
@@ -686,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,6 +762,26 @@
       </c>
       <c r="E2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45340</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -767,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,6 +1274,50 @@
       <c r="I18" s="2" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45341</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45340</v>
+      </c>
+      <c r="E20" s="4">
+        <v>400</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E24" s="4"/>

</xml_diff>

<commit_message>
Abrechnug geändert: Gewinn Getränke sowie Umsatz Spezialpreise
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F622BD-6A5B-4572-9D34-3E3CBF744FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF64372-FABC-4137-BB05-C04848D31C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="2565" windowWidth="21900" windowHeight="12435" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="2475" yWindow="3585" windowWidth="21900" windowHeight="12435" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Beitrag Stiftung Lebenshilfe</t>
+  </si>
+  <si>
+    <t>Einkauf Wein 1dl</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I20" totalsRowShown="0">
-  <autoFilter ref="A1:I20" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I16">
-    <sortCondition ref="A1:A16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I21" totalsRowShown="0">
+  <autoFilter ref="A1:I21" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
+    <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
@@ -806,10 +809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,19 +865,19 @@
         <v>45311</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1">
         <v>45311</v>
       </c>
       <c r="E2" s="4">
-        <v>75.849999999999994</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -884,19 +887,22 @@
         <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="E3" s="4">
-        <v>48.5</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -905,42 +911,42 @@
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5">
-        <v>45319</v>
+      <c r="B4" s="1">
+        <v>45312</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="5">
-        <v>45319</v>
+        <v>21</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45312</v>
       </c>
       <c r="E4" s="4">
-        <v>24</v>
+        <v>48.5</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45319</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1">
-        <v>45316</v>
+        <v>28</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45319</v>
       </c>
       <c r="E5" s="4">
-        <v>34.5</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -950,62 +956,61 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
-        <v>45331</v>
+        <v>45316</v>
       </c>
       <c r="E6" s="4">
-        <v>101</v>
+        <v>34.5</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1">
-        <v>45316</v>
+        <v>45331</v>
       </c>
       <c r="E7" s="4">
-        <v>32.700000000000003</v>
+        <v>101</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1">
         <v>45316</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" ref="E8:E9" si="0">1140*1.1</f>
-        <v>1254</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -1021,62 +1026,59 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45316</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" ref="E9:E10" si="0">1140*1.1</f>
+        <v>1254</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>45347</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>1254</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1">
-        <v>45330</v>
-      </c>
-      <c r="E10" s="4">
-        <v>100</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1">
-        <v>45329</v>
+        <v>45330</v>
       </c>
       <c r="E11" s="4">
-        <v>35.049999999999997</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
         <v>40</v>
@@ -1085,10 +1087,10 @@
         <v>41</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1096,52 +1098,49 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1">
-        <v>44895</v>
+        <v>45329</v>
       </c>
       <c r="E12" s="4">
-        <v>15.75</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>42491</v>
+        <v>41</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45311</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1">
-        <v>45330</v>
+        <v>44895</v>
       </c>
       <c r="E13" s="4">
-        <v>423.5</v>
+        <v>15.75</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <v>42491</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1149,28 +1148,28 @@
         <v>23</v>
       </c>
       <c r="B14" s="1">
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1">
-        <v>45329</v>
+        <v>45330</v>
       </c>
       <c r="E14" s="4">
-        <v>276.3</v>
+        <v>423.5</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,61 +1177,68 @@
         <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>45316</v>
+        <v>45312</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="E15" s="4">
-        <v>194.6</v>
+        <v>276.3</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45316</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1">
-        <v>45316</v>
+        <v>45321</v>
       </c>
       <c r="E16" s="4">
-        <v>1200</v>
+        <v>194.6</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1">
-        <v>45347</v>
+        <v>45316</v>
       </c>
       <c r="E17" s="4">
         <v>1200</v>
@@ -1248,79 +1254,101 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1">
-        <v>45333</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1">
-        <v>45337</v>
+        <v>45347</v>
       </c>
       <c r="E18" s="4">
-        <v>192.45</v>
+        <v>1200</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>45340</v>
+        <v>45333</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1">
-        <v>45341</v>
+        <v>45337</v>
       </c>
       <c r="E19" s="4">
-        <v>1000</v>
+        <v>192.45</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>45340</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1">
-        <v>45323</v>
+        <v>45341</v>
       </c>
       <c r="E20" s="4">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="4"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45340</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45323</v>
+      </c>
+      <c r="E21" s="4">
+        <v>400</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1335,7 +1363,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A165</xm:sqref>
+          <xm:sqref>A3:A166</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
neue Verleiherrechnung 10.02.24 Jakobs Ross
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894CE50D-2D02-4D18-9F9F-044636B01A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF133AB1-F6D3-4A90-AF5E-EFD3C6139F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="1215" windowWidth="21900" windowHeight="12435" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -275,6 +275,21 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>Film: Jakobs Ross</t>
+  </si>
+  <si>
+    <t>Elite Film AG</t>
+  </si>
+  <si>
+    <t>Seminarstrasse 28, 8057 Zürich</t>
+  </si>
+  <si>
+    <t>25 93110 00000 00000 00012 45132</t>
+  </si>
+  <si>
+    <t>00124513</t>
   </si>
 </sst>
 </file>
@@ -380,8 +395,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I21" totalsRowShown="0">
-  <autoFilter ref="A1:I21" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I22" totalsRowShown="0">
+  <autoFilter ref="A1:I22" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
     <sortCondition ref="A1:A17"/>
   </sortState>
@@ -712,22 +727,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -750,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -767,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -811,24 +826,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -857,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -882,7 +897,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -907,7 +922,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -929,7 +944,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -951,7 +966,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -973,7 +988,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -999,7 +1014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1036,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1059,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1082,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1172,7 +1187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1201,7 +1216,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1245,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1252,7 +1267,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1274,7 +1289,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1303,7 +1318,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1325,7 +1340,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1347,7 +1362,36 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1">
+        <v>37308</v>
+      </c>
+      <c r="E22" s="4">
+        <v>417.7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E25" s="4"/>
     </row>
   </sheetData>
@@ -1379,47 +1423,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Eintritte und Kiosk 20.3.24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FF15DD-95E1-439B-9622-EF19BD439640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0380D61-1527-4325-ACDA-FB9B1DC4E6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -731,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,6 +822,23 @@
         <v>240</v>
       </c>
       <c r="E4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45371</v>
+      </c>
+      <c r="D5" s="4">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Neue Rechnung und Verleiherabgaben
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0380D61-1527-4325-ACDA-FB9B1DC4E6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E37873-A6F9-41CD-800E-BDBDC4414691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15120" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>Kollekte</t>
+  </si>
+  <si>
+    <t>SKV Suisa Abgaben</t>
+  </si>
+  <si>
+    <t>00 00000 00000 01361 70105 86706</t>
+  </si>
+  <si>
+    <t>13617</t>
   </si>
 </sst>
 </file>
@@ -401,8 +410,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I23" totalsRowShown="0">
-  <autoFilter ref="A1:I23" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:I24" totalsRowShown="0">
+  <autoFilter ref="A1:I24" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
     <sortCondition ref="A1:A17"/>
   </sortState>
@@ -733,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -866,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1452,6 +1461,32 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45376</v>
+      </c>
+      <c r="E24" s="4">
+        <v>25.1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E25" s="4"/>

</xml_diff>

<commit_message>
neue Verleiherrechnung Jakobs Ross
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB2F6E1-4569-4552-90F2-FCFFA729932D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16C5FA-4E98-4039-B190-8A911137C165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="121">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Schokobrunnen Wonka</t>
   </si>
   <si>
-    <t>Stefan Jablonski</t>
-  </si>
-  <si>
     <t>Verleiher</t>
   </si>
   <si>
@@ -362,6 +359,48 @@
   </si>
   <si>
     <t>00085456</t>
+  </si>
+  <si>
+    <t>weischer.cinema Schweiz GmbH</t>
+  </si>
+  <si>
+    <t>Rämistrasse 6, 8001 Zürich</t>
+  </si>
+  <si>
+    <t>240277TS</t>
+  </si>
+  <si>
+    <t>Werbeiweischer Februar 2024</t>
+  </si>
+  <si>
+    <t>Werbeiweischer März 2024</t>
+  </si>
+  <si>
+    <t>240184TS</t>
+  </si>
+  <si>
+    <t>Funnyhouse Eventvermietungen</t>
+  </si>
+  <si>
+    <t>Engelbergstrasse 10, 6243 Egolzwil</t>
+  </si>
+  <si>
+    <t>4405</t>
+  </si>
+  <si>
+    <t>Einkauf Kioskwaren Kino</t>
+  </si>
+  <si>
+    <t>Filmmiete Kino</t>
+  </si>
+  <si>
+    <t>Film Jakobs Ross</t>
+  </si>
+  <si>
+    <t>25 93110 00000 00000 00012 65007</t>
+  </si>
+  <si>
+    <t>00126500</t>
   </si>
 </sst>
 </file>
@@ -408,13 +447,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,8 +500,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G6" totalsRowShown="0">
-  <autoFilter ref="A1:G6" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
     <sortCondition ref="E1:E2"/>
   </sortState>
@@ -478,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:J29" totalsRowShown="0">
-  <autoFilter ref="A1:J29" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:J31" totalsRowShown="0">
+  <autoFilter ref="A1:J31" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
     <sortCondition ref="A1:A17"/>
   </sortState>
@@ -809,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,7 +892,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -868,10 +909,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5">
         <v>45340</v>
@@ -880,18 +921,18 @@
         <v>1000</v>
       </c>
       <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
         <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="5">
         <v>45368</v>
@@ -900,15 +941,15 @@
         <v>240</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5">
         <v>45371</v>
@@ -917,7 +958,53 @@
         <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45390</v>
+      </c>
+      <c r="D6" s="4">
+        <v>16.29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45357</v>
+      </c>
+      <c r="D7" s="4">
+        <v>65.25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +1019,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A6</xm:sqref>
+          <xm:sqref>A2:A7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -942,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +1049,7 @@
     <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -991,18 +1078,18 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1">
         <v>45311</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1">
         <v>45311</v>
@@ -1014,15 +1101,15 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1">
         <v>45311</v>
@@ -1046,9 +1133,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1">
         <v>45312</v>
@@ -1060,24 +1147,33 @@
         <v>45312</v>
       </c>
       <c r="E4" s="4">
-        <v>48.5</v>
+        <v>52.45</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5">
         <v>45319</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5">
         <v>45319</v>
@@ -1086,13 +1182,13 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1115,12 +1211,12 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1">
         <v>45331</v>
@@ -1129,25 +1225,25 @@
         <v>101</v>
       </c>
       <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>45316</v>
@@ -1165,12 +1261,12 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1">
         <v>45316</v>
@@ -1189,12 +1285,12 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1">
         <v>45347</v>
@@ -1213,12 +1309,12 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1">
         <v>45330</v>
@@ -1227,25 +1323,25 @@
         <v>100</v>
       </c>
       <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>45329</v>
@@ -1254,25 +1350,25 @@
         <v>35.049999999999997</v>
       </c>
       <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
         <v>39</v>
       </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
       <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>49</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
       </c>
       <c r="D13" s="1">
         <v>44895</v>
@@ -1281,10 +1377,10 @@
         <v>15.75</v>
       </c>
       <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
         <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>52</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2">
@@ -1292,15 +1388,15 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>45311</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1">
         <v>45330</v>
@@ -1309,28 +1405,28 @@
         <v>423.5</v>
       </c>
       <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
         <v>34</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>45312</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1">
         <v>45329</v>
@@ -1339,28 +1435,28 @@
         <v>276.3</v>
       </c>
       <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
         <v>43</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>45316</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1">
         <v>45321</v>
@@ -1369,25 +1465,25 @@
         <v>194.6</v>
       </c>
       <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
         <v>53</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1">
         <v>45316</v>
@@ -1399,18 +1495,18 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1">
         <v>45347</v>
@@ -1422,21 +1518,21 @@
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>45333</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1">
         <v>45337</v>
@@ -1445,28 +1541,28 @@
         <v>192.45</v>
       </c>
       <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
         <v>66</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>67</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>45340</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1">
         <v>45341</v>
@@ -1475,21 +1571,21 @@
         <v>1000</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1">
         <v>45340</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1">
         <v>45323</v>
@@ -1498,21 +1594,21 @@
         <v>400</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>45332</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1">
         <v>37308</v>
@@ -1521,28 +1617,28 @@
         <v>417.7</v>
       </c>
       <c r="F22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" t="s">
         <v>80</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1">
         <v>45354</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1">
         <v>45354</v>
@@ -1551,18 +1647,18 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1">
         <v>45376</v>
@@ -1571,30 +1667,34 @@
         <v>25.1</v>
       </c>
       <c r="F24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" t="s">
         <v>39</v>
       </c>
-      <c r="G24" t="s">
-        <v>40</v>
-      </c>
       <c r="H24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>45344</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="1">
         <v>45387</v>
@@ -1603,30 +1703,34 @@
         <v>205.4</v>
       </c>
       <c r="F25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" t="s">
         <v>90</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="J25" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
         <v>45368</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" s="1">
         <v>45387</v>
@@ -1635,30 +1739,34 @@
         <v>178.35</v>
       </c>
       <c r="F26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" t="s">
         <v>66</v>
       </c>
-      <c r="G26" t="s">
-        <v>67</v>
-      </c>
       <c r="H26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1">
         <v>45386</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1">
         <v>45387</v>
@@ -1667,30 +1775,34 @@
         <v>139.75</v>
       </c>
       <c r="F27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
         <v>66</v>
       </c>
-      <c r="G27" t="s">
-        <v>67</v>
-      </c>
       <c r="H27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J27" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
         <v>45354</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="1">
         <v>45387</v>
@@ -1699,54 +1811,110 @@
         <v>137.9</v>
       </c>
       <c r="F28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" t="s">
         <v>66</v>
       </c>
-      <c r="G28" t="s">
-        <v>67</v>
-      </c>
       <c r="H28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1">
         <v>45358</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="1">
-        <v>5.0423999999999998</v>
+        <v>45387</v>
       </c>
       <c r="E29" s="4">
         <v>104</v>
       </c>
       <c r="F29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" t="s">
         <v>66</v>
       </c>
-      <c r="G29" t="s">
-        <v>67</v>
-      </c>
       <c r="H29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="J29" s="2" t="s">
-        <v>95</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45339</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45392</v>
+      </c>
+      <c r="E30" s="4">
+        <v>461.95</v>
+      </c>
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D31" s="1"/>
+      <c r="E31" s="4"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1759,7 +1927,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A167</xm:sqref>
+          <xm:sqref>A3:A168</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1782,12 +1950,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -1802,12 +1970,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Errorhandling meherer Filme für einen Tag eingetragen in Verleiherabrechnung
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16C5FA-4E98-4039-B190-8A911137C165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46D2EA4-838C-4840-B616-B0853C128A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="122">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>00126500</t>
+  </si>
+  <si>
+    <t>Buchungskonto Name</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -508,8 +514,8 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
     <tableColumn id="2" xr3:uid="{4A3D2615-9D9C-4A35-9563-6454B477091D}" name="Bezeichnung"/>
-    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{EC0FDCA3-B34E-4378-9B61-6671AF218B0B}" name="Firmennamen"/>
     <tableColumn id="8" xr3:uid="{359B982D-E085-4831-8FE0-859B1B4314AD}" name="Adresse"/>
     <tableColumn id="10" xr3:uid="{02367AEA-A5FC-4D0B-90AF-F9D0D56EB4A0}" name="Rechnungsnummer"/>
@@ -519,22 +525,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:J31" totalsRowShown="0">
-  <autoFilter ref="A1:J31" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K31" totalsRowShown="0">
+  <autoFilter ref="A1:K31" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
-    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum" dataDxfId="6"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
-    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{0C538012-5D92-4E64-B81F-85CAF66FE963}" name="Firmennamen"/>
     <tableColumn id="5" xr3:uid="{528DBE91-75A0-4B49-8AC8-06D027A50035}" name="Adresse"/>
-    <tableColumn id="6" xr3:uid="{4B5E1481-D849-49CA-8C98-0F7393B356B7}" name="Referenz" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{9ADB258D-2FDB-4B52-85E7-8DAB899CA101}" name="Buchungskonto" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4B5E1481-D849-49CA-8C98-0F7393B356B7}" name="Referenz" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{9B01639A-96D8-4A50-B1D3-C69E9C49B9DA}" name="Buchungskonto" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{9ADB258D-2FDB-4B52-85E7-8DAB899CA101}" name="Buchungskonto Name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1029,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L1:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,10 +1053,11 @@
     <col min="7" max="7" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1080,8 +1088,11 @@
       <c r="J1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1106,8 +1117,9 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1132,8 +1144,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1160,12 +1173,13 @@
       <c r="J4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="2" t="s">
         <v>116</v>
       </c>
       <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1187,8 +1201,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1210,8 +1225,9 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1237,8 +1253,9 @@
         <v>32</v>
       </c>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1260,8 +1277,9 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1284,8 +1302,9 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1308,8 +1327,9 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1335,8 +1355,9 @@
         <v>41</v>
       </c>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1362,8 +1383,9 @@
         <v>48</v>
       </c>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1387,8 +1409,9 @@
         <v>42491</v>
       </c>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1417,8 +1440,9 @@
         <v>36</v>
       </c>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1447,8 +1471,9 @@
         <v>45</v>
       </c>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1477,8 +1502,9 @@
         <v>55</v>
       </c>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1500,8 +1526,9 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1523,8 +1550,9 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1553,8 +1581,9 @@
         <v>68</v>
       </c>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1576,8 +1605,9 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -1599,8 +1629,9 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1629,8 +1660,9 @@
         <v>82</v>
       </c>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1652,8 +1684,9 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1681,12 +1714,13 @@
       <c r="J24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1717,12 +1751,13 @@
       <c r="J25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1753,12 +1788,13 @@
       <c r="J26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1789,12 +1825,13 @@
       <c r="J27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="K27" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1825,12 +1862,13 @@
       <c r="J28" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1861,12 +1899,13 @@
       <c r="J29" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="2" t="s">
         <v>117</v>
       </c>
       <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1897,23 +1936,25 @@
       <c r="J30" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
       <c r="E31" s="4"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Neue Verleiherrechung Ella 1.4.24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46D2EA4-838C-4840-B616-B0853C128A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D792BE-5F7C-46AC-906E-6A25849BEE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="125">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>Buchungskonto Name</t>
+  </si>
+  <si>
+    <t>Film: Ella und der schwarze Jaguar</t>
+  </si>
+  <si>
+    <t>25 93110 00000 00000 00012 67012</t>
+  </si>
+  <si>
+    <t>00126701</t>
   </si>
 </sst>
 </file>
@@ -540,8 +549,8 @@
     <tableColumn id="5" xr3:uid="{528DBE91-75A0-4B49-8AC8-06D027A50035}" name="Adresse"/>
     <tableColumn id="6" xr3:uid="{4B5E1481-D849-49CA-8C98-0F7393B356B7}" name="Referenz" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{64D50181-342C-4387-875F-8ADB060C0EDC}" name="Rechnungsnummer" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{9B01639A-96D8-4A50-B1D3-C69E9C49B9DA}" name="Buchungskonto" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{9ADB258D-2FDB-4B52-85E7-8DAB899CA101}" name="Buchungskonto Name" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9B01639A-96D8-4A50-B1D3-C69E9C49B9DA}" name="Buchungskonto" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{9ADB258D-2FDB-4B52-85E7-8DAB899CA101}" name="Buchungskonto Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1038,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L1:M29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1939,12 +1948,39 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D31" s="1"/>
-      <c r="E31" s="4"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45394</v>
+      </c>
+      <c r="E31" s="4">
+        <v>211.9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Der Wert der Dinge Veranstaltung 06.04.24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9262D1-B787-4491-B102-C4E356078798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABEB74-F692-4B34-867D-6ABDD929E059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -428,6 +428,15 @@
   </si>
   <si>
     <t>ROB_014</t>
+  </si>
+  <si>
+    <t>Film: Der Wert der Dinge</t>
+  </si>
+  <si>
+    <t>Tobias Luchsinger</t>
+  </si>
+  <si>
+    <t>Merkurstrasse 27</t>
   </si>
 </sst>
 </file>
@@ -549,8 +558,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K32" totalsRowShown="0">
-  <autoFilter ref="A1:K32" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K33" totalsRowShown="0">
+  <autoFilter ref="A1:K33" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
     <sortCondition ref="A1:A17"/>
   </sortState>
@@ -887,18 +896,18 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -921,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -938,7 +947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -958,7 +967,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -975,7 +984,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1060,28 +1069,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1143,7 +1152,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1170,7 +1179,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1203,7 +1212,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1227,7 +1236,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1260,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1279,7 +1288,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1303,7 +1312,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1328,7 +1337,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1353,7 +1362,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1390,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1409,7 +1418,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1435,7 +1444,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1466,7 +1475,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1497,7 +1506,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1528,7 +1537,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1552,7 +1561,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1576,7 +1585,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1607,7 +1616,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1631,7 +1640,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -1655,7 +1664,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1695,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1710,7 +1719,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1744,7 +1753,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1781,7 +1790,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1818,7 +1827,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1855,7 +1864,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1892,7 +1901,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1929,7 +1938,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1962,7 +1971,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1997,7 +2006,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2029,6 +2038,37 @@
         <v>94</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45418</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45387</v>
+      </c>
+      <c r="E33" s="4">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2070,47 +2110,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Neue Verleiherrechnungen erhalten, Wert der Dinge, Beyond Tradition, Hors Normes, La Chimera, The Hypnosis
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B965152B-966C-4833-ADE0-B1B1415DF7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F3FE5-57A0-423A-9051-B1BF003D30DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="154">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -467,6 +467,39 @@
   </si>
   <si>
     <t>Kinomiete Mai</t>
+  </si>
+  <si>
+    <t>Film: La Chimera</t>
+  </si>
+  <si>
+    <t>93 64950 00000 00000 00008 61717</t>
+  </si>
+  <si>
+    <t>00086171</t>
+  </si>
+  <si>
+    <t>Film: Hors Normes</t>
+  </si>
+  <si>
+    <t>25 93110 00000 00000 00012 82338</t>
+  </si>
+  <si>
+    <t>00128233</t>
+  </si>
+  <si>
+    <t>Film: The Hypnosis</t>
+  </si>
+  <si>
+    <t>45713</t>
+  </si>
+  <si>
+    <t>Film: Beyond Tradition</t>
+  </si>
+  <si>
+    <t>ExtraMileFilms GmbH</t>
+  </si>
+  <si>
+    <t>Bachweg 16, 9631 Ulisbach</t>
   </si>
 </sst>
 </file>
@@ -588,10 +621,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K40" totalsRowShown="0">
-  <autoFilter ref="A1:K40" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K40">
-    <sortCondition ref="C1:C40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K43" totalsRowShown="0">
+  <autoFilter ref="A1:K43" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K42">
+    <sortCondition ref="F1:F42"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
@@ -1139,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,82 +1230,91 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45344</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1">
-        <v>45329</v>
+        <v>45387</v>
       </c>
       <c r="E2" s="4">
-        <v>35.049999999999997</v>
+        <v>205.4</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45354</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1">
-        <v>44895</v>
+        <v>45354</v>
       </c>
       <c r="E3" s="4">
-        <v>15.75</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2">
-        <v>42491</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>45311</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1">
-        <v>45311</v>
+        <v>45330</v>
       </c>
       <c r="E4" s="4">
-        <v>75.849999999999994</v>
+        <v>423.5</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="7"/>
@@ -1280,25 +1322,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45311</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>45311</v>
+        <v>45316</v>
       </c>
       <c r="E5" s="4">
-        <v>60</v>
+        <v>34.5</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1343,91 +1382,95 @@
         <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>45344</v>
+        <v>45332</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D7" s="1">
-        <v>45387</v>
+        <v>37308</v>
       </c>
       <c r="E7" s="4">
-        <v>205.4</v>
+        <v>417.7</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>45311</v>
+        <v>45371</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>146</v>
       </c>
       <c r="D8" s="1">
-        <v>45330</v>
+        <v>45422</v>
       </c>
       <c r="E8" s="4">
-        <v>423.5</v>
+        <v>162.15</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>35</v>
+        <v>147</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>45418</v>
+        <v>45383</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D9" s="1">
-        <v>45387</v>
+        <v>45394</v>
       </c>
       <c r="E9" s="4">
-        <v>170</v>
+        <v>211.9</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>92</v>
       </c>
@@ -1440,47 +1483,51 @@
         <v>22</v>
       </c>
       <c r="B10" s="1">
-        <v>45316</v>
+        <v>45386</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D10" s="1">
-        <v>45321</v>
+        <v>45387</v>
       </c>
       <c r="E10" s="4">
-        <v>194.6</v>
+        <v>139.75</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1">
-        <v>45383</v>
+        <v>45358</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1">
-        <v>45394</v>
+        <v>45387</v>
       </c>
       <c r="E11" s="4">
-        <v>211.9</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
         <v>63</v>
@@ -1489,10 +1536,10 @@
         <v>64</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>92</v>
@@ -1506,16 +1553,16 @@
         <v>22</v>
       </c>
       <c r="B12" s="1">
-        <v>45386</v>
+        <v>45333</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1">
-        <v>45387</v>
+        <v>45337</v>
       </c>
       <c r="E12" s="4">
-        <v>139.75</v>
+        <v>192.45</v>
       </c>
       <c r="F12" t="s">
         <v>63</v>
@@ -1523,34 +1570,30 @@
       <c r="G12" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>97</v>
+      <c r="H12" t="s">
+        <v>65</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>45358</v>
+        <v>45368</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1">
         <v>45387</v>
       </c>
       <c r="E13" s="4">
-        <v>104</v>
+        <v>178.35</v>
       </c>
       <c r="F13" t="s">
         <v>63</v>
@@ -1559,10 +1602,10 @@
         <v>64</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>92</v>
@@ -1576,220 +1619,200 @@
         <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>45332</v>
+        <v>45354</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1">
-        <v>37308</v>
+        <v>45387</v>
       </c>
       <c r="E14" s="4">
-        <v>417.7</v>
+        <v>137.9</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>45340</v>
+        <v>45415</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="D15" s="1">
-        <v>45341</v>
+        <v>45426</v>
       </c>
       <c r="E15" s="4">
-        <v>1000</v>
+        <v>137.9</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1">
-        <v>45403</v>
+        <v>45312</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1">
-        <v>45403</v>
+        <v>45312</v>
       </c>
       <c r="E16" s="4">
-        <v>447.55</v>
+        <v>52.45</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>92</v>
+        <v>112</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1">
-        <v>45333</v>
+        <v>45340</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1">
-        <v>45337</v>
+        <v>45323</v>
       </c>
       <c r="E17" s="4">
-        <v>192.45</v>
+        <v>400</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1">
-        <v>45368</v>
+        <v>45311</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1">
-        <v>45387</v>
+        <v>45311</v>
       </c>
       <c r="E18" s="4">
-        <v>178.35</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1">
-        <v>45354</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1">
-        <v>45387</v>
+        <v>45347</v>
       </c>
       <c r="E19" s="4">
-        <v>137.9</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45312</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1">
-        <v>45329</v>
+        <v>45316</v>
       </c>
       <c r="E20" s="4">
-        <v>276.3</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -1798,10 +1821,10 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1">
-        <v>45347</v>
+        <v>45376</v>
       </c>
       <c r="E21" s="4">
         <f>1140*1.1</f>
@@ -1823,10 +1846,10 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="D22" s="1">
-        <v>45316</v>
+        <v>45407</v>
       </c>
       <c r="E22" s="4">
         <f>1140*1.1</f>
@@ -1848,13 +1871,13 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D23" s="1">
-        <v>45376</v>
+        <v>45437</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" ref="E23:E25" si="0">1140*1.1</f>
+        <f>1140*1.1</f>
         <v>1254</v>
       </c>
       <c r="F23" t="s">
@@ -1870,17 +1893,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1">
-        <v>45407</v>
+        <v>45316</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
@@ -1895,28 +1917,38 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45403</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D25" s="1">
-        <v>45437</v>
+        <v>45403</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>447.55</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1944,25 +1976,29 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="1">
-        <v>45354</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1">
-        <v>45354</v>
+        <v>45329</v>
       </c>
       <c r="E27" s="4">
-        <v>10</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="7"/>
@@ -1970,25 +2006,29 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1">
-        <v>45316</v>
+        <v>45330</v>
       </c>
       <c r="E28" s="4">
-        <v>34.5</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="7"/>
@@ -1996,42 +2036,53 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1">
-        <v>45316</v>
+        <v>45376</v>
       </c>
       <c r="E29" s="4">
-        <v>32.700000000000003</v>
+        <v>25.1</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>75</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45311</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="D30" s="1">
-        <v>45316</v>
+        <v>45311</v>
       </c>
       <c r="E30" s="4">
-        <v>1200</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -2051,10 +2102,10 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" s="1">
-        <v>45347</v>
+        <v>45316</v>
       </c>
       <c r="E31" s="4">
         <v>1200</v>
@@ -2077,10 +2128,10 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" s="1">
-        <v>45376</v>
+        <v>45347</v>
       </c>
       <c r="E32" s="4">
         <v>1200</v>
@@ -2103,10 +2154,10 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" s="1">
-        <v>45407</v>
+        <v>45376</v>
       </c>
       <c r="E33" s="4">
         <v>1200</v>
@@ -2127,10 +2178,10 @@
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="1">
-        <v>45437</v>
+        <v>45407</v>
       </c>
       <c r="E34" s="4">
         <v>1200</v>
@@ -2151,47 +2202,43 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1">
-        <v>45330</v>
+        <v>45437</v>
       </c>
       <c r="E35" s="4">
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1">
         <v>45340</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1">
-        <v>45323</v>
+        <v>45341</v>
       </c>
       <c r="E36" s="4">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2200,100 +2247,682 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>45312</v>
+        <v>45418</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="D37" s="1">
-        <v>45312</v>
+        <v>45387</v>
       </c>
       <c r="E37" s="4">
-        <v>52.45</v>
+        <v>170</v>
       </c>
       <c r="F37" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="G37" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="6" t="s">
-        <v>113</v>
+      <c r="J37" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45316</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D38" s="1">
-        <v>45376</v>
+        <v>45321</v>
       </c>
       <c r="E38" s="4">
-        <v>25.1</v>
+        <v>194.6</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G38" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45312</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D39" s="1">
-        <v>45331</v>
+        <v>45329</v>
       </c>
       <c r="E39" s="4">
-        <v>101</v>
+        <v>276.3</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G39" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="1">
+        <v>44895</v>
+      </c>
+      <c r="E40" s="4">
+        <v>15.75</v>
+      </c>
+      <c r="F40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" t="s">
+        <v>51</v>
+      </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="I40" s="2">
+        <v>42491</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45400</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="1">
+        <v>45400</v>
+      </c>
+      <c r="E41" s="4">
+        <v>211.85</v>
+      </c>
+      <c r="F41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45331</v>
+      </c>
+      <c r="E42" s="4">
+        <v>101</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45319</v>
+      </c>
+      <c r="C43" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="1">
+        <v>45421</v>
+      </c>
+      <c r="E43" s="4">
+        <v>179.08</v>
+      </c>
+      <c r="F43" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" t="s">
+        <v>153</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E112" s="4"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E113" s="4"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E117" s="4"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E118" s="4"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E119" s="4"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E120" s="4"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E121" s="4"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E123" s="4"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E124" s="4"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E125" s="4"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E126" s="4"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E127" s="4"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E128" s="4"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E130" s="4"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E137" s="4"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E138" s="4"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E139" s="4"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E140" s="4"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E141" s="4"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E142" s="4"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E143" s="4"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E146" s="4"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E149" s="4"/>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E150" s="4"/>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E153" s="4"/>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E154" s="4"/>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E155" s="4"/>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E158" s="4"/>
+    </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E159" s="4"/>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E160" s="4"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E161" s="4"/>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E162" s="4"/>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E163" s="4"/>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E164" s="4"/>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E165" s="4"/>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E166" s="4"/>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E167" s="4"/>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E168" s="4"/>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E169" s="4"/>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E170" s="4"/>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E171" s="4"/>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E172" s="4"/>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E174" s="4"/>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E175" s="4"/>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E177" s="4"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E178" s="4"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E179" s="4"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E180" s="4"/>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E181" s="4"/>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E182" s="4"/>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E183" s="4"/>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E188" s="4"/>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E189" s="4"/>
+    </row>
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E190" s="4"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E191" s="4"/>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E192" s="4"/>
+    </row>
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E193" s="4"/>
+    </row>
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E194" s="4"/>
+    </row>
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E195" s="4"/>
+    </row>
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E196" s="4"/>
+    </row>
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E197" s="4"/>
+    </row>
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E198" s="4"/>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E199" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2317,7 +2946,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A41:A168 A3:A39</xm:sqref>
+          <xm:sqref>A42:A169 A3:A39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Kinovorstellung Perfect Days 2305.24 und Rechnung All of us strangers
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F3FE5-57A0-423A-9051-B1BF003D30DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D928EAC1-96B9-494F-837C-6090078F9FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="158">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -500,6 +500,18 @@
   </si>
   <si>
     <t>Bachweg 16, 9631 Ulisbach</t>
+  </si>
+  <si>
+    <t>Film: All of us strangers</t>
+  </si>
+  <si>
+    <t>The Walt Disney Company Switzerland</t>
+  </si>
+  <si>
+    <t>Stampfenbachstrasse 48, 8006 Zürich</t>
+  </si>
+  <si>
+    <t>376416</t>
   </si>
 </sst>
 </file>
@@ -621,8 +633,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K43" totalsRowShown="0">
-  <autoFilter ref="A1:K43" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K44" totalsRowShown="0">
+  <autoFilter ref="A1:K44" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K42">
     <sortCondition ref="F1:F42"/>
   </sortState>
@@ -1174,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2457,7 +2469,37 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E44" s="4"/>
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45428</v>
+      </c>
+      <c r="C44" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="1">
+        <v>45435</v>
+      </c>
+      <c r="E44" s="4">
+        <v>227.55</v>
+      </c>
+      <c r="F44" t="s">
+        <v>155</v>
+      </c>
+      <c r="G44" t="s">
+        <v>156</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E45" s="4"/>

</xml_diff>

<commit_message>
Rechnung alll of us stranger datum angepasst
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D928EAC1-96B9-494F-837C-6090078F9FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00655B1A-4E59-4571-B4C2-25A32DB83B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2473,7 +2473,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="1">
-        <v>45428</v>
+        <v>45431</v>
       </c>
       <c r="C44" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
Verleiherrechnung Perfect Days 23.05.24 und Werbungskosten Schabi
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00655B1A-4E59-4571-B4C2-25A32DB83B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C78D48C-AE41-46D7-A0F3-EAE90DED5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="169">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -512,6 +512,39 @@
   </si>
   <si>
     <t>376416</t>
+  </si>
+  <si>
+    <t>Film: Perfect Days</t>
+  </si>
+  <si>
+    <t>03019739</t>
+  </si>
+  <si>
+    <t>96 57660 00000 00000 00301 97392</t>
+  </si>
+  <si>
+    <t>Druckkosten Monatsprogram Jan-Mai 24</t>
+  </si>
+  <si>
+    <t>Stefan Jablonski</t>
+  </si>
+  <si>
+    <t>Sonnhaldenstrasse 13, 5734 Reinach AG</t>
+  </si>
+  <si>
+    <t>Gestaltung Porgramm und Dias</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>4406</t>
+  </si>
+  <si>
+    <t>Werbung Kino</t>
   </si>
 </sst>
 </file>
@@ -558,13 +591,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -633,8 +667,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K44" totalsRowShown="0">
-  <autoFilter ref="A1:K44" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K47" totalsRowShown="0">
+  <autoFilter ref="A1:K47" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K42">
     <sortCondition ref="F1:F42"/>
   </sortState>
@@ -1187,7 +1221,7 @@
   <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,63 +2536,151 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E45" s="4"/>
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45435</v>
+      </c>
+      <c r="C45" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="1">
+        <v>45439</v>
+      </c>
+      <c r="E45" s="4">
+        <v>253.55</v>
+      </c>
+      <c r="F45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" t="s">
+        <v>34</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E46" s="4"/>
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45435</v>
+      </c>
+      <c r="E46" s="4">
+        <v>479.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" t="s">
+        <v>163</v>
+      </c>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E47" s="4"/>
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="1">
+        <v>45435</v>
+      </c>
+      <c r="E47" s="4">
+        <v>420</v>
+      </c>
+      <c r="F47" t="s">
+        <v>162</v>
+      </c>
+      <c r="G47" t="s">
+        <v>163</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.3">
@@ -2967,7 +3089,7 @@
       <c r="E199" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="L4:M4"/>
@@ -2975,6 +3097,7 @@
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="L30:M30"/>
+    <mergeCell ref="K50:L50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Migros Support Culture Beitrag
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C78D48C-AE41-46D7-A0F3-EAE90DED5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3BF7F3-D7CA-4F6E-9AB9-B3D2A00BB820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="172">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -545,6 +545,15 @@
   </si>
   <si>
     <t>Werbung Kino</t>
+  </si>
+  <si>
+    <t>Vermietung Impuls Zusammenleben The Old Oak</t>
+  </si>
+  <si>
+    <t>Vermietung Impuls Zusammenleben Hors Normes</t>
+  </si>
+  <si>
+    <t>Migros Support Culture</t>
   </si>
 </sst>
 </file>
@@ -591,14 +600,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -648,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G9" totalsRowShown="0">
-  <autoFilter ref="A1:G9" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
     <sortCondition ref="E1:E2"/>
   </sortState>
@@ -669,8 +677,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K47" totalsRowShown="0">
   <autoFilter ref="A1:K47" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K42">
-    <sortCondition ref="F1:F42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
+    <sortCondition ref="C1:C47"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
@@ -999,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,6 +1204,57 @@
         <v>134</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45368</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45371</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45439</v>
+      </c>
+      <c r="D12" s="4">
+        <v>977.6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1208,7 +1267,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A9</xm:sqref>
+          <xm:sqref>A2:A12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1220,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView topLeftCell="A16" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,114 +1335,111 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45344</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
-        <v>45387</v>
+        <v>45329</v>
       </c>
       <c r="E2" s="4">
-        <v>205.4</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45354</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1">
-        <v>45354</v>
+        <v>44895</v>
       </c>
       <c r="E3" s="4">
-        <v>10</v>
+        <v>15.75</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2">
+        <v>42491</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45311</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="D4" s="1">
-        <v>45330</v>
+        <v>45435</v>
       </c>
       <c r="E4" s="4">
-        <v>423.5</v>
+        <v>479.5</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>75</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45311</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
-        <v>45316</v>
+        <v>45311</v>
       </c>
       <c r="E5" s="4">
-        <v>34.5</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1392,35 +1448,29 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1">
-        <v>45339</v>
+        <v>45311</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1">
-        <v>45392</v>
+        <v>45311</v>
       </c>
       <c r="E6" s="4">
-        <v>461.95</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1428,16 +1478,16 @@
         <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>45332</v>
+        <v>45339</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="D7" s="1">
-        <v>37308</v>
+        <v>45392</v>
       </c>
       <c r="E7" s="4">
-        <v>417.7</v>
+        <v>461.95</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
@@ -1446,12 +1496,14 @@
         <v>78</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1459,28 +1511,26 @@
         <v>22</v>
       </c>
       <c r="B8" s="1">
-        <v>45371</v>
+        <v>45431</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D8" s="1">
-        <v>45422</v>
+        <v>45435</v>
       </c>
       <c r="E8" s="4">
-        <v>162.15</v>
+        <v>227.55</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>147</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>92</v>
@@ -1494,28 +1544,28 @@
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>45383</v>
+        <v>45344</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1">
-        <v>45394</v>
+        <v>45387</v>
       </c>
       <c r="E9" s="4">
-        <v>211.9</v>
+        <v>205.4</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>92</v>
@@ -1529,29 +1579,25 @@
         <v>22</v>
       </c>
       <c r="B10" s="1">
-        <v>45386</v>
+        <v>45319</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="D10" s="1">
-        <v>45387</v>
+        <v>45421</v>
       </c>
       <c r="E10" s="4">
-        <v>139.75</v>
+        <v>179.08</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>98</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
         <v>92</v>
       </c>
@@ -1564,117 +1610,109 @@
         <v>22</v>
       </c>
       <c r="B11" s="1">
-        <v>45358</v>
+        <v>45311</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1">
-        <v>45387</v>
+        <v>45330</v>
       </c>
       <c r="E11" s="4">
-        <v>104</v>
+        <v>423.5</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1">
-        <v>45333</v>
+        <v>45418</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="D12" s="1">
-        <v>45337</v>
+        <v>45387</v>
       </c>
       <c r="E12" s="4">
-        <v>192.45</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>45368</v>
+        <v>45316</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1">
-        <v>45387</v>
+        <v>45321</v>
       </c>
       <c r="E13" s="4">
-        <v>178.35</v>
+        <v>194.6</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>45354</v>
+        <v>45383</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1">
-        <v>45387</v>
+        <v>45394</v>
       </c>
       <c r="E14" s="4">
-        <v>137.9</v>
+        <v>211.9</v>
       </c>
       <c r="F14" t="s">
         <v>63</v>
@@ -1683,10 +1721,10 @@
         <v>64</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>92</v>
@@ -1700,16 +1738,16 @@
         <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>45415</v>
+        <v>45386</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="D15" s="1">
-        <v>45426</v>
+        <v>45387</v>
       </c>
       <c r="E15" s="4">
-        <v>137.9</v>
+        <v>139.75</v>
       </c>
       <c r="F15" t="s">
         <v>63</v>
@@ -1718,10 +1756,10 @@
         <v>64</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>92</v>
@@ -1732,155 +1770,193 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
-        <v>45312</v>
+        <v>45358</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="D16" s="1">
-        <v>45312</v>
+        <v>45387</v>
       </c>
       <c r="E16" s="4">
-        <v>52.45</v>
+        <v>104</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="6" t="s">
-        <v>113</v>
+        <v>64</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>45340</v>
+        <v>45371</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1">
-        <v>45323</v>
+        <v>45422</v>
       </c>
       <c r="E17" s="4">
-        <v>400</v>
+        <v>162.15</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>45311</v>
+        <v>45332</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1">
-        <v>45311</v>
+        <v>37308</v>
       </c>
       <c r="E18" s="4">
-        <v>75.849999999999994</v>
+        <v>417.7</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45415</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="D19" s="1">
-        <v>45347</v>
+        <v>45426</v>
       </c>
       <c r="E19" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>137.9</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45435</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="D20" s="1">
-        <v>45316</v>
+        <v>45439</v>
       </c>
       <c r="E20" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>253.55</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45340</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="D21" s="1">
-        <v>45376</v>
+        <v>45341</v>
       </c>
       <c r="E21" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>1000</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1889,105 +1965,130 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45403</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D22" s="1">
-        <v>45407</v>
+        <v>45403</v>
       </c>
       <c r="E22" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>447.55</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45333</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1">
-        <v>45437</v>
+        <v>45337</v>
       </c>
       <c r="E23" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>192.45</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45400</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="D24" s="1">
-        <v>45316</v>
+        <v>45400</v>
       </c>
       <c r="E24" s="4">
-        <v>32.700000000000003</v>
+        <v>211.85</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>45403</v>
+        <v>45368</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="D25" s="1">
-        <v>45403</v>
+        <v>45387</v>
       </c>
       <c r="E25" s="4">
-        <v>447.55</v>
+        <v>178.35</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G25" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>92</v>
@@ -1998,52 +2099,66 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="5">
-        <v>45319</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45354</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="5">
-        <v>45319</v>
+        <v>99</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45387</v>
       </c>
       <c r="E26" s="4">
-        <v>24</v>
+        <v>137.9</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45312</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D27" s="1">
         <v>45329</v>
       </c>
       <c r="E27" s="4">
-        <v>35.049999999999997</v>
+        <v>276.3</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -2052,29 +2167,26 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>136</v>
       </c>
       <c r="D28" s="1">
-        <v>45330</v>
+        <v>45407</v>
       </c>
       <c r="E28" s="4">
-        <v>100</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="7"/>
@@ -2082,59 +2194,50 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1">
-        <v>45376</v>
+        <v>45347</v>
       </c>
       <c r="E29" s="4">
-        <v>25.1</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="1">
-        <v>45311</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D30" s="1">
-        <v>45311</v>
+        <v>45316</v>
       </c>
       <c r="E30" s="4">
-        <v>60</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2145,22 +2248,23 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1">
-        <v>45316</v>
+        <v>45437</v>
       </c>
       <c r="E31" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2171,22 +2275,23 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D32" s="1">
-        <v>45347</v>
+        <v>45376</v>
       </c>
       <c r="E32" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2197,46 +2302,52 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="D33" s="1">
-        <v>45376</v>
+        <v>45435</v>
       </c>
       <c r="E33" s="4">
-        <v>1200</v>
+        <v>420</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="I33" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>75</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45354</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="D34" s="1">
-        <v>45407</v>
+        <v>45354</v>
       </c>
       <c r="E34" s="4">
-        <v>1200</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2245,22 +2356,22 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="5">
+        <v>45319</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="5">
+        <v>45319</v>
+      </c>
+      <c r="E35" s="4">
         <v>24</v>
       </c>
-      <c r="C35" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="1">
-        <v>45437</v>
-      </c>
-      <c r="E35" s="4">
-        <v>1200</v>
-      </c>
       <c r="F35" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2269,22 +2380,22 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="1">
-        <v>45340</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1">
-        <v>45341</v>
+        <v>45316</v>
       </c>
       <c r="E36" s="4">
-        <v>1000</v>
+        <v>34.5</v>
       </c>
       <c r="F36" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2293,94 +2404,73 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="1">
-        <v>45418</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="D37" s="1">
-        <v>45387</v>
+        <v>45316</v>
       </c>
       <c r="E37" s="4">
-        <v>170</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F37" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="1">
-        <v>45316</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="D38" s="1">
-        <v>45321</v>
+        <v>45407</v>
       </c>
       <c r="E38" s="4">
-        <v>194.6</v>
+        <v>1200</v>
       </c>
       <c r="F38" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45312</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="D39" s="1">
-        <v>45329</v>
+        <v>45347</v>
       </c>
       <c r="E39" s="4">
-        <v>276.3</v>
+        <v>1200</v>
       </c>
       <c r="F39" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>43</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
@@ -2389,246 +2479,215 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="D40" s="1">
-        <v>44895</v>
+        <v>45316</v>
       </c>
       <c r="E40" s="4">
-        <v>15.75</v>
+        <v>1200</v>
       </c>
       <c r="F40" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="2">
-        <v>42491</v>
-      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="1">
-        <v>45400</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D41" s="1">
-        <v>45400</v>
+        <v>45437</v>
       </c>
       <c r="E41" s="4">
-        <v>211.85</v>
+        <v>1200</v>
       </c>
       <c r="F41" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H41" s="2"/>
-      <c r="I41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="D42" s="1">
-        <v>45331</v>
+        <v>45376</v>
       </c>
       <c r="E42" s="4">
-        <v>101</v>
+        <v>1200</v>
       </c>
       <c r="F42" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1">
-        <v>45319</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="D43" s="1">
-        <v>45421</v>
+        <v>45330</v>
       </c>
       <c r="E43" s="4">
-        <v>179.08</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="G43" t="s">
-        <v>153</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B44" s="1">
-        <v>45431</v>
+        <v>45340</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="D44" s="1">
-        <v>45435</v>
+        <v>45323</v>
       </c>
       <c r="E44" s="4">
-        <v>227.55</v>
+        <v>400</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
       <c r="H44" s="2"/>
-      <c r="I44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B45" s="1">
-        <v>45435</v>
+        <v>45312</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>21</v>
       </c>
       <c r="D45" s="1">
-        <v>45439</v>
+        <v>45312</v>
       </c>
       <c r="E45" s="4">
-        <v>253.55</v>
+        <v>52.45</v>
       </c>
       <c r="F45" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>92</v>
+        <v>112</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="D46" s="1">
-        <v>45435</v>
+        <v>45376</v>
       </c>
       <c r="E46" s="4">
-        <v>479.5</v>
+        <v>25.1</v>
       </c>
       <c r="F46" t="s">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>163</v>
-      </c>
-      <c r="H46" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="I46" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>167</v>
+        <v>85</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>28</v>
       </c>
       <c r="D47" s="1">
-        <v>45435</v>
+        <v>45331</v>
       </c>
       <c r="E47" s="4">
-        <v>420</v>
+        <v>101</v>
       </c>
       <c r="F47" t="s">
-        <v>162</v>
+        <v>29</v>
       </c>
       <c r="G47" t="s">
-        <v>163</v>
-      </c>
-      <c r="H47" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I47" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>168</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E48" s="4"/>
@@ -3090,6 +3149,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K50:L50"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="L4:M4"/>
@@ -3097,7 +3157,6 @@
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="L30:M30"/>
-    <mergeCell ref="K50:L50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
neue Ausgaben / Einnahmen (SKV, Werbeweischer)
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A7BF35-11C5-47EA-944E-F484397CAA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F8288-589E-4065-AB1C-72F08C2A6172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="183">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -563,6 +563,30 @@
   </si>
   <si>
     <t>Haupstrasse 93, 5737 Menziken</t>
+  </si>
+  <si>
+    <t>00 00000 00000 01343 00105 86707</t>
+  </si>
+  <si>
+    <t>13430</t>
+  </si>
+  <si>
+    <t>Werbeweischer Mai 2024</t>
+  </si>
+  <si>
+    <t>240484TS</t>
+  </si>
+  <si>
+    <t>SKV Suisa Abgaben Akonto 1. Quartal</t>
+  </si>
+  <si>
+    <t>SKV Suisa Abgaben Akonto 2. Quartal</t>
+  </si>
+  <si>
+    <t>13944</t>
+  </si>
+  <si>
+    <t>00 00000 00000 01394 40105 86708</t>
   </si>
 </sst>
 </file>
@@ -665,8 +689,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G13" totalsRowShown="0">
-  <autoFilter ref="A1:G13" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
     <sortCondition ref="A1:A13"/>
   </sortState>
@@ -684,8 +708,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K47" totalsRowShown="0">
-  <autoFilter ref="A1:K47" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K49" totalsRowShown="0">
+  <autoFilter ref="A1:K49" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1016,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,6 +1308,29 @@
         <v>174</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45448</v>
+      </c>
+      <c r="D14" s="4">
+        <v>26.01</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1296,7 +1343,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A13</xm:sqref>
+          <xm:sqref>A2:A14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1309,7 +1356,7 @@
   <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2719,56 +2766,114 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" s="1">
+        <v>45352</v>
+      </c>
+      <c r="E48" s="4">
+        <v>51.45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="1">
+        <v>45444</v>
+      </c>
+      <c r="E49" s="4">
+        <v>80.150000000000006</v>
+      </c>
+      <c r="F49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E50" s="4"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Verleiherrechnung Coup de Chance
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanjablonski/Documents/Kinoklub_Finance/Kinoklub/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCD841F-0F8B-4E25-B03B-B76AE899028C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17B8493-85FC-654B-A74D-BAA284C81CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="192">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -606,15 +606,25 @@
   </si>
   <si>
     <t>Glace: Gitziberghof</t>
+  </si>
+  <si>
+    <t>Film: Coup de  Chance</t>
+  </si>
+  <si>
+    <t>Riedtlistrasse 23, 8001 Zürich</t>
+  </si>
+  <si>
+    <t>10052051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -676,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -687,10 +697,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -709,10 +720,10 @@
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
@@ -753,8 +764,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K51" totalsRowShown="0">
-  <autoFilter ref="A1:K51" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K52" totalsRowShown="0">
+  <autoFilter ref="A1:K52" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -789,9 +800,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,7 +840,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -935,7 +946,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,7 +1088,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1091,18 +1102,18 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1145,7 +1156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1179,7 +1190,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1196,7 +1207,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1213,7 +1224,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1247,7 +1258,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1264,7 +1275,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1298,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1310,7 +1321,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1344,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1364,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1398,28 +1409,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:M198"/>
+  <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49:K49"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1454,7 +1465,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1481,7 +1492,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1508,7 +1519,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1534,7 +1545,7 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1558,7 +1569,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1582,7 +1593,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1613,7 +1624,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1637,7 +1648,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1661,7 +1672,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1700,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1725,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1739,7 +1750,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1764,7 +1775,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1789,7 +1800,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1814,7 +1825,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1842,7 +1853,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1868,7 +1879,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1892,7 +1903,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1916,7 +1927,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1940,7 +1951,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1964,7 +1975,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1988,7 +1999,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2016,7 +2027,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2048,7 +2059,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2081,7 +2092,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2114,7 +2125,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2151,7 +2162,7 @@
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2184,7 +2195,7 @@
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2217,7 +2228,7 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2250,7 +2261,7 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2283,7 +2294,7 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2320,7 +2331,7 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2355,7 +2366,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2390,7 +2401,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2425,7 +2436,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2456,7 +2467,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2491,7 +2502,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2526,7 +2537,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2550,7 +2561,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2585,7 +2596,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2616,7 +2627,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2649,7 +2660,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2684,7 +2695,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2719,7 +2730,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2750,7 +2761,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2780,7 +2791,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2810,7 +2821,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -2842,7 +2853,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -2874,7 +2885,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -2893,7 +2904,7 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2917,466 +2928,520 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D52" s="1"/>
-      <c r="E52" s="4"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D53" s="1"/>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45412</v>
+      </c>
+      <c r="C52" t="s">
+        <v>189</v>
+      </c>
+      <c r="D52" s="1">
+        <v>45460</v>
+      </c>
+      <c r="E52" s="4">
+        <v>214</v>
+      </c>
+      <c r="F52" t="s">
+        <v>185</v>
+      </c>
+      <c r="G52" t="s">
+        <v>190</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B53" s="10"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="4"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D54" s="1"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B54" s="10"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="4"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D55" s="1"/>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B55" s="10"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="4"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D56" s="1"/>
       <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D57" s="1"/>
       <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D58" s="1"/>
       <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E68" s="4"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E69" s="4"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E198" s="4"/>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E199" s="4"/>
+    </row>
+    <row r="200" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E200" s="4"/>
+    </row>
+    <row r="201" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E201" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3400,7 +3465,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A39 A42:A168</xm:sqref>
+          <xm:sqref>A3:A39 A42:A171</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3416,9 +3481,9 @@
       <selection activeCell="K3" sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -3435,7 +3500,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3470,7 +3535,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3521,47 +3586,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Fehlermeldung Kategorien Event/Verleiher angepasst
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA55D4A5-5DC9-4C7C-809B-6B0A849C41EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEE6FB2-AC75-4F22-85CD-8985A5157C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2879,6 +2879,9 @@
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>75</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45332</v>
       </c>
       <c r="C50" t="s">
         <v>183</v>
@@ -3465,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFEBA5D-FF22-4032-BB29-794CF56A632B}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rechnung Resilient Man eingetroffen
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841615BC-2B4D-4F8B-B2F9-0BFCC7B5BE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C97CC5-BEDA-455F-A6BC-B338A74F650F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="222">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -695,6 +695,15 @@
   </si>
   <si>
     <t>1000540408</t>
+  </si>
+  <si>
+    <t>Film:Resilient Man</t>
+  </si>
+  <si>
+    <t>93 64950 00000 00000 00008 81501</t>
+  </si>
+  <si>
+    <t>00088150</t>
   </si>
 </sst>
 </file>
@@ -842,8 +851,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K59" totalsRowShown="0">
-  <autoFilter ref="A1:K59" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K60" totalsRowShown="0">
+  <autoFilter ref="A1:K60" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1489,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3276,7 +3285,39 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E60" s="4"/>
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45562</v>
+      </c>
+      <c r="C60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D60" s="1">
+        <v>45568</v>
+      </c>
+      <c r="E60" s="4">
+        <v>88.85</v>
+      </c>
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E61" s="4"/>

</xml_diff>

<commit_message>
Film: La passion de Dodin Buffant (06.10.24) und Garfield (08.09.24) eingetragen.
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C97CC5-BEDA-455F-A6BC-B338A74F650F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDF452C-27AF-4039-852E-3B770023696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="5112" yWindow="5220" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1498,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ausgaben Tschugger - Raclette Rechnung
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FB9C34-9BE6-411B-AB99-EE7F94DB6148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F9831-CEE9-43DD-904C-0FCF98A6F17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="234">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -715,7 +715,31 @@
     <t>Raclette-Stand: Gurken &amp; Silberzwiebeln</t>
   </si>
   <si>
-    <t>Raclette-Stand: Käse und Racletteofen</t>
+    <t>Raclette-Stand: Weisswein Wallis</t>
+  </si>
+  <si>
+    <t>Raclette-Stand:Raclette - Nachschub</t>
+  </si>
+  <si>
+    <t>ZauberSpiess: Schokolade und Spiesse</t>
+  </si>
+  <si>
+    <t>Raclette-Stand: Käse und Racletteofen Rechnung Käserei</t>
+  </si>
+  <si>
+    <t>Chäsparadies Seengen</t>
+  </si>
+  <si>
+    <t>Poststrasse 23, 5707 Seengen</t>
+  </si>
+  <si>
+    <t>87 25020 00002 59330 00000 58102</t>
+  </si>
+  <si>
+    <t>25933</t>
+  </si>
+  <si>
+    <t>Spesen</t>
   </si>
 </sst>
 </file>
@@ -726,7 +750,7 @@
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,6 +767,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -793,7 +823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -803,8 +833,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,8 +902,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K65" totalsRowShown="0">
-  <autoFilter ref="A1:K65" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K67" totalsRowShown="0">
+  <autoFilter ref="A1:K67" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1519,7 +1550,7 @@
   <dimension ref="A1:M201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,8 +1680,8 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2266,8 +2297,8 @@
       <c r="K27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2299,8 +2330,8 @@
       <c r="K28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2332,8 +2363,8 @@
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -2365,8 +2396,8 @@
       <c r="K30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -2398,8 +2429,8 @@
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -2435,8 +2466,8 @@
       <c r="K32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -3358,7 +3389,9 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
+      <c r="K61" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -3379,7 +3412,9 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
+      <c r="K62" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -3389,18 +3424,20 @@
         <v>45576</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D63" s="1">
         <v>45576</v>
       </c>
       <c r="E63" s="4">
-        <v>200</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
+      <c r="K63" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -3416,12 +3453,14 @@
         <v>45576</v>
       </c>
       <c r="E64" s="4">
-        <v>200</v>
+        <v>102.2</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
+      <c r="K64" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -3430,25 +3469,79 @@
       <c r="B65" s="1">
         <v>45576</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>225</v>
+      <c r="C65" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="D65" s="1">
+        <v>45579</v>
+      </c>
+      <c r="E65" s="4">
+        <v>279.89999999999998</v>
+      </c>
+      <c r="F65" t="s">
+        <v>229</v>
+      </c>
+      <c r="G65" t="s">
+        <v>230</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="1">
         <v>45576</v>
       </c>
-      <c r="E65" s="4">
-        <v>300</v>
-      </c>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E66" s="4"/>
+      <c r="C66" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45576</v>
+      </c>
+      <c r="E66" s="4">
+        <v>30.7</v>
+      </c>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E67" s="4"/>
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45578</v>
+      </c>
+      <c r="C67" t="s">
+        <v>227</v>
+      </c>
+      <c r="D67" s="1">
+        <v>45578</v>
+      </c>
+      <c r="E67" s="4">
+        <v>50.25</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E68" s="4"/>

</xml_diff>

<commit_message>
Eintritte & Kiosk 18.10.24, Tschugger Verleiherrechnung, FördererFilm Andrea
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F9831-CEE9-43DD-904C-0FCF98A6F17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6301CB00-8DF6-42A1-8B98-0FFA7D175E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="6156" yWindow="6264" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="241">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -740,6 +740,27 @@
   </si>
   <si>
     <t>Spesen</t>
+  </si>
+  <si>
+    <t>Film:Andrea lässt sich scheiden</t>
+  </si>
+  <si>
+    <t>93 64950 00000 00000 00008 86095</t>
+  </si>
+  <si>
+    <t>00088609</t>
+  </si>
+  <si>
+    <t>Fördereranlass</t>
+  </si>
+  <si>
+    <t>Film: Tschugger (beide)</t>
+  </si>
+  <si>
+    <t>25 93110 00000 00000 00013 27334</t>
+  </si>
+  <si>
+    <t>00132733</t>
   </si>
 </sst>
 </file>
@@ -902,8 +923,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K67" totalsRowShown="0">
-  <autoFilter ref="A1:K67" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K69" totalsRowShown="0">
+  <autoFilter ref="A1:K69" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1549,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="H53" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3544,10 +3565,72 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E68" s="4"/>
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45581</v>
+      </c>
+      <c r="C68" t="s">
+        <v>234</v>
+      </c>
+      <c r="D68" s="1">
+        <v>45583</v>
+      </c>
+      <c r="E68" s="4">
+        <v>232.4</v>
+      </c>
+      <c r="F68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G68" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E69" s="4"/>
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="1">
+        <v>45577</v>
+      </c>
+      <c r="C69" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" s="1">
+        <v>45583</v>
+      </c>
+      <c r="E69" s="4">
+        <v>924.65</v>
+      </c>
+      <c r="F69" t="s">
+        <v>77</v>
+      </c>
+      <c r="G69" t="s">
+        <v>78</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E70" s="4"/>

</xml_diff>

<commit_message>
corrected kategorie in Einnahmen und Ausgaben.xlsx
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6301CB00-8DF6-42A1-8B98-0FFA7D175E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC692C93-FB91-443C-8194-C3B119030458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6156" yWindow="6264" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -859,8 +859,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -959,9 +959,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -999,7 +999,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1105,7 +1105,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1261,18 +1261,18 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1570,26 +1570,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H53" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1678,7 +1678,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1884,7 +1884,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1934,7 +1934,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2110,7 +2110,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2420,7 +2420,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2626,7 +2626,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3564,9 +3564,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B68" s="1">
         <v>45581</v>
@@ -3597,9 +3597,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B69" s="1">
         <v>45577</v>
@@ -3632,400 +3632,400 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E201" s="4"/>
     </row>
   </sheetData>
@@ -4066,47 +4066,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Neue Rechnungen - Dodin und DSDMT3
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A036DB-DB36-4FEE-BF95-C9B5F88E6421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC2D43A-B02E-484A-8EB0-C84EC95146E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="17544" yWindow="0" windowWidth="13272" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="249">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -770,6 +770,21 @@
   </si>
   <si>
     <t>Impuls Zusammenleben aargauSüd</t>
+  </si>
+  <si>
+    <t>Film: Die Schule der Magischen Tiere 3</t>
+  </si>
+  <si>
+    <t>96 57660 00000 00000 00302 08784</t>
+  </si>
+  <si>
+    <t>03020878</t>
+  </si>
+  <si>
+    <t>Film: La Passion de Dodin Bouffant</t>
+  </si>
+  <si>
+    <t>26 27680 00000 00000 01005 30821</t>
   </si>
 </sst>
 </file>
@@ -932,8 +947,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K69" totalsRowShown="0">
-  <autoFilter ref="A1:K69" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K71" totalsRowShown="0">
+  <autoFilter ref="A1:K71" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1266,7 +1281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1599,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3662,10 +3677,74 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E70" s="4"/>
+      <c r="A70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="1">
+        <v>45578</v>
+      </c>
+      <c r="C70" t="s">
+        <v>244</v>
+      </c>
+      <c r="D70" s="1">
+        <v>45589</v>
+      </c>
+      <c r="E70" s="4">
+        <v>194.6</v>
+      </c>
+      <c r="F70" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E71" s="4"/>
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="1">
+        <v>45571</v>
+      </c>
+      <c r="C71" t="s">
+        <v>247</v>
+      </c>
+      <c r="D71" s="1">
+        <v>45588</v>
+      </c>
+      <c r="E71" s="4">
+        <v>181.6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>184</v>
+      </c>
+      <c r="G71" t="s">
+        <v>188</v>
+      </c>
+      <c r="H71" t="s">
+        <v>248</v>
+      </c>
+      <c r="I71" s="2">
+        <v>10053082</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E72" s="4"/>

</xml_diff>